<commit_message>
Updated packages comparison spreadsheet.
</commit_message>
<xml_diff>
--- a/php-sysinfo-packages-comparison.xlsx
+++ b/php-sysinfo-packages-comparison.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Packages Overview" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Packages API Comparison" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,9 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
-  <si>
-    <t xml:space="preserve">URL</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
+  <si>
+    <t xml:space="preserve">g</t>
   </si>
   <si>
     <t xml:space="preserve">Last Commit</t>
@@ -75,22 +76,13 @@
     <t xml:space="preserve">Test Windows Support</t>
   </si>
   <si>
-    <t xml:space="preserve">https://packagist.org/packages/danielme85/simple-server-info</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feb 05 2020</t>
+    <t xml:space="preserve">https://github.com/Gemorroj/ginfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 31 2019</t>
   </si>
   <si>
     <t xml:space="preserve">7.1+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No windows support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Gemorroj/ginfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec 31 2019</t>
   </si>
   <si>
     <t xml:space="preserve">symfony/process: "^4.2|^5.0"</t>
@@ -103,6 +95,382 @@
   <si>
     <t xml:space="preserve">Fork of linfo/linfo. Better php 7+ architecture
 Linux and Windows &gt;= 10 only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ginfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trntv/probe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Architecture:   E.g x86_64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getCPUArchitecture()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser-&gt;getGeneral(): General</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getArchitecture(): string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of Logical / Virtual Processors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">count($parser→getCPU())</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$info→getCpu()→getVirtual()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getCpuCores(): int|null</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Cpu Model e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Intel(R) Core(TM) i5-3570 CPU @ 3.40GHz</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getCPU()[$i]['Model']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$info-&gt;getCpu()-&gt;getProcessors()[$i]-&gt;getModel(): string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getCpuModel(): string|null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of Physical CPU Cores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$info→getCpu()→getCores()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getCpuPhysicalCores(): int|null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cpu Core Usage Percentages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">array_column($parser→getCPU()[$i], ‘usage_percentage’)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getCpuUsage(): array</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Cpu Vendor E.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">GenuineIntel</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$parser→getCPU()[$i]['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Vendor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">']</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$info→getCpu()→getProcessors()[$i]→getAllProcessorInfo()[‘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">vendor_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">’]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getCpuVendor(): string|null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free Ram (bytes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getRam()[‘free’]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getMemory()→getFree()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getFreeMem(): int|null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free Swap Memory (bytes)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$parser→getRam()[‘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">swapFree</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">’]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getMemory()→getSwapFree()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getFreeSwap(): int|null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Host-name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getHostName()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getGeneral()→getHostname()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider→getHostname()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kernel Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getKernel()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getGeneral()→getKernel()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getOsKernelVersion(): mixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distro Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getDistro()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getGeneral()→getOsName()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getOsRelease(): mixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OS Family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getOS()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getOsType(): mixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getPhp()→getDisabledFunctions()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getPhpDisabledFunctions(): array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getPhpInfo(): string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getPhp()→getExtensions(): array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getPhpModules(): array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getPhp()→getSapiName(): string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getPhpSapiName(): mixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getPhpVersion()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getPhp()→getVersion(): string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getPhpVersion(): string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Ram (bytes)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$parser→getRam()[‘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">total</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">’]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getMemory()→getTotal(): float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getTotalMem(): int|null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Swap Memory (bytes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getRam()[‘swapTotal’]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getMemory()→getSwapTotal(): ?float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getTotalSwap(): int|null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uptime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getUpTime()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getGeneral()→getUptime(): ?\DateInterval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used Ram (bytes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getMemory()→getUsed(): float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getUsedMem(): int|null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used  Swap Memory (bytes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getMemory()→getSwapUsed(): ?float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getUsedSwap(): int|null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$parser→getWebService()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$provider-&gt;getServerSoftware(): mixed</t>
   </si>
 </sst>
 </file>
@@ -112,7 +480,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -152,10 +520,70 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibiri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val=""/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -210,7 +638,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,6 +664,46 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -317,17 +785,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="3" sqref="C2 C10:C12 C21 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.52"/>
@@ -398,11 +866,11 @@
         <v>10</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="31.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -410,48 +878,27 @@
         <v>18</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="31.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="n">
-        <v>19</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://packagist.org/packages/linfo/linfo"/>
     <hyperlink ref="A3" r:id="rId2" display="https://packagist.org/packages/trntv/probe"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://packagist.org/packages/danielme85/simple-server-info"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://github.com/Gemorroj/ginfo"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://github.com/Gemorroj/ginfo"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -461,4 +908,325 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ24"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="2" sqref="C2 C10:C12 C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="52.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="53.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="65.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="41.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.76"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>